<commit_message>
Add Visual Corner Post
</commit_message>
<xml_diff>
--- a/assets/xls/Weight Loss.xlsx
+++ b/assets/xls/Weight Loss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\minima\assets\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AFF6DD-7EE6-40A1-B309-1604E911EEE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8022E3F2-9181-4CD8-A223-6790864C02E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3375,7 +3375,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="14213D"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="14213D"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Average Monthly Weight (kgs)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="14213D"/>
+              </a:solidFill>
+              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3383,9 +3438,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="2.868738425925926E-2"/>
-          <c:y val="0.14296029332356372"/>
+          <c:y val="8.4885195444752218E-2"/>
           <c:w val="0.93868101851851837"/>
-          <c:h val="0.70985266140814729"/>
+          <c:h val="0.76792771402189663"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3406,7 +3461,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="14213D"/>
               </a:solidFill>
@@ -3416,12 +3471,12 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="9"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:srgbClr val="CEA03B"/>
               </a:solidFill>
-              <a:ln w="12700">
+              <a:ln w="19050">
                 <a:solidFill>
                   <a:srgbClr val="14213D"/>
                 </a:solidFill>
@@ -3808,7 +3863,9 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:noFill/>
+    <a:solidFill>
+      <a:srgbClr val="FFFAEB"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -3830,7 +3887,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -6043,15 +6099,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>312125</xdr:colOff>
+      <xdr:colOff>312124</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>128221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>244325</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>98971</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>118428</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3721</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6286,190 +6342,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.00092</cdr:x>
-      <cdr:y>0</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>1</cdr:x>
-      <cdr:y>0.09931</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 15">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DF5923-E925-49FE-9437-52BA7944CAA9}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8259" y="0"/>
-          <a:ext cx="8968550" cy="540000"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr val="14213D"/>
-        </a:solidFill>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </cdr:style>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Average</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Monthly Weight (kgs)</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -6956,17 +6828,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W210"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="W38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AI35" sqref="AI35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.9296875" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7019,7 +6891,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -7093,7 +6965,7 @@
         <v>26.95</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -7167,7 +7039,7 @@
         <v>27.517241379310345</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7241,7 +7113,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -7315,7 +7187,7 @@
         <v>28.310344827586206</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -7389,7 +7261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -7463,7 +7335,7 @@
         <v>29.823529411764707</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -7537,7 +7409,7 @@
         <v>30.166666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -7611,7 +7483,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -7685,7 +7557,7 @@
         <v>30.666666666666668</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -7759,7 +7631,7 @@
         <v>30.714285714285715</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -7833,7 +7705,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -7907,7 +7779,7 @@
         <v>29.833333333333332</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -7981,7 +7853,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -8055,7 +7927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -8129,7 +8001,7 @@
         <v>30.533333333333335</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -8203,7 +8075,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -8262,7 +8134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -8321,7 +8193,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -8380,7 +8252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -8439,7 +8311,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -8498,7 +8370,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -8557,7 +8429,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -8616,7 +8488,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -8675,7 +8547,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -8734,7 +8606,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -8793,7 +8665,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -8852,7 +8724,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -8911,7 +8783,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -8970,7 +8842,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -9029,7 +8901,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -9088,7 +8960,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -9147,7 +9019,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -9206,7 +9078,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -9265,7 +9137,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -9324,7 +9196,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -9383,7 +9255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -9442,7 +9314,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -9501,7 +9373,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -9560,7 +9432,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -9619,7 +9491,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>92</v>
       </c>
@@ -9678,7 +9550,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -9737,7 +9609,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -9796,7 +9668,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -9855,7 +9727,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -9914,7 +9786,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>102</v>
       </c>
@@ -9973,7 +9845,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -10032,7 +9904,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -10091,7 +9963,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -10150,7 +10022,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -10209,7 +10081,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -10268,7 +10140,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -10327,7 +10199,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -10386,7 +10258,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>116</v>
       </c>
@@ -10445,7 +10317,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>117</v>
       </c>
@@ -10504,7 +10376,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>118</v>
       </c>
@@ -10563,7 +10435,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -10622,7 +10494,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -10681,7 +10553,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -10740,7 +10612,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>124</v>
       </c>
@@ -10799,7 +10671,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -10858,7 +10730,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -10917,7 +10789,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -10976,7 +10848,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -11035,7 +10907,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -11094,7 +10966,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -11153,7 +11025,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -11212,7 +11084,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -11271,7 +11143,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>142</v>
       </c>
@@ -11330,7 +11202,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -11389,7 +11261,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -11448,7 +11320,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>148</v>
       </c>
@@ -11507,7 +11379,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -11566,7 +11438,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -11625,7 +11497,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>151</v>
       </c>
@@ -11684,7 +11556,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>153</v>
       </c>
@@ -11743,7 +11615,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -11802,7 +11674,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>155</v>
       </c>
@@ -11861,7 +11733,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -11920,7 +11792,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>161</v>
       </c>
@@ -11979,7 +11851,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -12038,7 +11910,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -12097,7 +11969,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -12156,7 +12028,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>169</v>
       </c>
@@ -12215,7 +12087,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>172</v>
       </c>
@@ -12274,7 +12146,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>173</v>
       </c>
@@ -12333,7 +12205,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -12392,7 +12264,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>175</v>
       </c>
@@ -12451,7 +12323,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -12510,7 +12382,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -12569,7 +12441,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>178</v>
       </c>
@@ -12628,7 +12500,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>179</v>
       </c>
@@ -12687,7 +12559,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>180</v>
       </c>
@@ -12746,7 +12618,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -12805,7 +12677,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>186</v>
       </c>
@@ -12864,7 +12736,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>188</v>
       </c>
@@ -12923,7 +12795,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>189</v>
       </c>
@@ -12982,7 +12854,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>193</v>
       </c>
@@ -13041,7 +12913,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>197</v>
       </c>
@@ -13100,7 +12972,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>202</v>
       </c>
@@ -13159,7 +13031,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>203</v>
       </c>
@@ -13218,7 +13090,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -13277,7 +13149,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>205</v>
       </c>
@@ -13336,7 +13208,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>206</v>
       </c>
@@ -13395,7 +13267,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -13454,7 +13326,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>209</v>
       </c>
@@ -13513,7 +13385,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>210</v>
       </c>
@@ -13572,7 +13444,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>211</v>
       </c>
@@ -13631,7 +13503,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -13690,7 +13562,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>216</v>
       </c>
@@ -13749,7 +13621,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>219</v>
       </c>
@@ -13808,7 +13680,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>221</v>
       </c>
@@ -13867,7 +13739,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>223</v>
       </c>
@@ -13926,7 +13798,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>224</v>
       </c>
@@ -13985,7 +13857,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>225</v>
       </c>
@@ -14044,7 +13916,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>227</v>
       </c>
@@ -14103,7 +13975,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>229</v>
       </c>
@@ -14162,7 +14034,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>231</v>
       </c>
@@ -14221,7 +14093,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>234</v>
       </c>
@@ -14280,7 +14152,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>235</v>
       </c>
@@ -14339,7 +14211,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>236</v>
       </c>
@@ -14398,7 +14270,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>237</v>
       </c>
@@ -14457,7 +14329,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>239</v>
       </c>
@@ -14516,7 +14388,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>240</v>
       </c>
@@ -14575,7 +14447,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>241</v>
       </c>
@@ -14634,7 +14506,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>243</v>
       </c>
@@ -14693,7 +14565,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>244</v>
       </c>
@@ -14752,7 +14624,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>245</v>
       </c>
@@ -14811,7 +14683,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>246</v>
       </c>
@@ -14870,7 +14742,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>250</v>
       </c>
@@ -14929,7 +14801,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>253</v>
       </c>
@@ -14988,7 +14860,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>258</v>
       </c>
@@ -15047,7 +14919,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>259</v>
       </c>
@@ -15106,7 +14978,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>261</v>
       </c>
@@ -15165,7 +15037,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>264</v>
       </c>
@@ -15224,7 +15096,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>267</v>
       </c>
@@ -15283,7 +15155,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>271</v>
       </c>
@@ -15342,7 +15214,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>272</v>
       </c>
@@ -15401,7 +15273,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>273</v>
       </c>
@@ -15460,7 +15332,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>275</v>
       </c>
@@ -15519,7 +15391,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>276</v>
       </c>
@@ -15578,7 +15450,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>280</v>
       </c>
@@ -15637,7 +15509,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>281</v>
       </c>
@@ -15696,7 +15568,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>284</v>
       </c>
@@ -15755,7 +15627,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>285</v>
       </c>
@@ -15814,7 +15686,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>287</v>
       </c>
@@ -15873,7 +15745,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>289</v>
       </c>
@@ -15932,7 +15804,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>290</v>
       </c>
@@ -15991,7 +15863,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>292</v>
       </c>
@@ -16050,7 +15922,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>293</v>
       </c>
@@ -16109,7 +15981,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>297</v>
       </c>
@@ -16168,7 +16040,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>300</v>
       </c>
@@ -16227,7 +16099,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>301</v>
       </c>
@@ -16286,7 +16158,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>302</v>
       </c>
@@ -16345,7 +16217,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>304</v>
       </c>
@@ -16404,7 +16276,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>305</v>
       </c>
@@ -16463,7 +16335,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>307</v>
       </c>
@@ -16522,7 +16394,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>309</v>
       </c>
@@ -16581,7 +16453,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>311</v>
       </c>
@@ -16640,7 +16512,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>312</v>
       </c>
@@ -16699,7 +16571,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>313</v>
       </c>
@@ -16758,7 +16630,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>314</v>
       </c>
@@ -16817,7 +16689,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>317</v>
       </c>
@@ -16876,7 +16748,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>320</v>
       </c>
@@ -16935,7 +16807,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>321</v>
       </c>
@@ -16994,7 +16866,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>323</v>
       </c>
@@ -17053,7 +16925,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>324</v>
       </c>
@@ -17112,7 +16984,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>325</v>
       </c>
@@ -17171,7 +17043,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>329</v>
       </c>
@@ -17230,7 +17102,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>330</v>
       </c>
@@ -17289,7 +17161,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>333</v>
       </c>
@@ -17348,7 +17220,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>335</v>
       </c>
@@ -17407,7 +17279,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>336</v>
       </c>
@@ -17466,7 +17338,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>337</v>
       </c>
@@ -17525,7 +17397,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>339</v>
       </c>
@@ -17584,7 +17456,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>340</v>
       </c>
@@ -17643,7 +17515,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>342</v>
       </c>
@@ -17702,7 +17574,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>343</v>
       </c>
@@ -17761,7 +17633,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>344</v>
       </c>
@@ -17820,7 +17692,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>345</v>
       </c>
@@ -17879,7 +17751,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>346</v>
       </c>
@@ -17938,7 +17810,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>347</v>
       </c>
@@ -17997,7 +17869,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>348</v>
       </c>
@@ -18056,7 +17928,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>351</v>
       </c>
@@ -18115,7 +17987,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>355</v>
       </c>
@@ -18174,7 +18046,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>357</v>
       </c>
@@ -18233,7 +18105,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>358</v>
       </c>
@@ -18292,7 +18164,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>359</v>
       </c>
@@ -18351,7 +18223,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>360</v>
       </c>
@@ -18410,7 +18282,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>362</v>
       </c>
@@ -18469,7 +18341,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>364</v>
       </c>
@@ -18528,7 +18400,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>367</v>
       </c>
@@ -18587,7 +18459,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>368</v>
       </c>
@@ -18646,7 +18518,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>369</v>
       </c>
@@ -18705,7 +18577,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>370</v>
       </c>
@@ -18764,7 +18636,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>371</v>
       </c>
@@ -18823,7 +18695,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>372</v>
       </c>
@@ -18882,7 +18754,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>373</v>
       </c>
@@ -18941,7 +18813,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>376</v>
       </c>
@@ -19000,7 +18872,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>379</v>
       </c>
@@ -19059,7 +18931,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>381</v>
       </c>
@@ -19118,7 +18990,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>382</v>
       </c>
@@ -19177,7 +19049,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>384</v>
       </c>
@@ -19236,7 +19108,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>385</v>
       </c>
@@ -19295,7 +19167,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>386</v>
       </c>
@@ -19354,7 +19226,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>387</v>
       </c>
@@ -19413,7 +19285,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>388</v>
       </c>
@@ -19472,7 +19344,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>390</v>
       </c>
@@ -19531,7 +19403,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>391</v>
       </c>

</xml_diff>